<commit_message>
tried new functionality with program.py
</commit_message>
<xml_diff>
--- a/input/example_input.xlsx
+++ b/input/example_input.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hannah\GoogleScraper\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahnguyen/Downloads/DHH/GoogleScraper/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8696510D-B03B-E34F-8D8C-AA3C11EAAE97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="504" windowWidth="28044" windowHeight="15936"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,17 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -40,9 +30,6 @@
     <t>AQC Traffic control</t>
   </si>
   <si>
-    <t>Organization</t>
-  </si>
-  <si>
     <t>Location</t>
   </si>
   <si>
@@ -71,19 +58,28 @@
   </si>
   <si>
     <t>Custom software</t>
+  </si>
+  <si>
+    <t>Firm Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -118,8 +114,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -455,72 +452,72 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="44" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="32" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.81640625" style="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="2" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>

</xml_diff>